<commit_message>
data update day 147
</commit_message>
<xml_diff>
--- a/covid19Naija/data/records_covid19.xlsx
+++ b/covid19Naija/data/records_covid19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="340" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="940" yWindow="420" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="records" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>Dates</t>
   </si>
@@ -460,8 +460,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -595,7 +637,7 @@
     <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -659,6 +701,27 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -722,6 +785,27 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1051,11 +1135,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP145"/>
+  <dimension ref="A1:AP155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A148" sqref="A148:AO148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9500,7 +9584,7 @@
         <v>2</v>
       </c>
       <c r="AO67">
-        <f t="shared" ref="AO67:AO129" si="1">SUM(B67:AL67)</f>
+        <f t="shared" ref="AO67:AO148" si="1">SUM(B67:AL67)</f>
         <v>87</v>
       </c>
     </row>
@@ -17317,36 +17401,38 @@
       </c>
     </row>
     <row r="130" spans="1:41">
-      <c r="A130" s="1"/>
+      <c r="A130" s="1">
+        <v>44009.654710648145</v>
+      </c>
       <c r="B130">
-        <v>0</v>
+        <v>285</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F130">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G130">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H130">
         <v>0</v>
       </c>
       <c r="I130">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J130">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K130">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="L130">
         <v>0</v>
@@ -17358,37 +17444,37 @@
         <v>0</v>
       </c>
       <c r="O130">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="P130">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q130">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R130">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="S130">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="T130">
         <v>0</v>
       </c>
       <c r="U130">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="V130">
         <v>0</v>
       </c>
       <c r="W130">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X130">
         <v>0</v>
       </c>
       <c r="Y130">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Z130">
         <v>0</v>
@@ -17403,79 +17489,85 @@
         <v>0</v>
       </c>
       <c r="AD130">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AE130">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF130">
         <v>0</v>
       </c>
       <c r="AG130">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH130">
         <v>0</v>
       </c>
       <c r="AI130">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ130">
         <v>0</v>
       </c>
       <c r="AK130">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="AL130">
         <v>0</v>
       </c>
       <c r="AM130">
-        <v>0</v>
+        <v>372</v>
       </c>
       <c r="AN130">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="AO130">
+        <f t="shared" si="1"/>
+        <v>779</v>
       </c>
     </row>
     <row r="131" spans="1:41">
-      <c r="A131" s="1"/>
+      <c r="A131" s="1">
+        <v>44010.644861111112</v>
+      </c>
       <c r="B131">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F131">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G131">
         <v>0</v>
       </c>
       <c r="H131">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I131">
         <v>0</v>
       </c>
       <c r="J131">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L131">
         <v>0</v>
       </c>
       <c r="M131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O131">
         <v>0</v>
@@ -17484,19 +17576,19 @@
         <v>0</v>
       </c>
       <c r="Q131">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R131">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="S131">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T131">
         <v>0</v>
       </c>
       <c r="U131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V131">
         <v>0</v>
@@ -17517,19 +17609,19 @@
         <v>0</v>
       </c>
       <c r="AB131">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AC131">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AD131">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AE131">
         <v>0</v>
       </c>
       <c r="AF131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG131">
         <v>0</v>
@@ -17541,52 +17633,58 @@
         <v>0</v>
       </c>
       <c r="AJ131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK131">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="AL131">
         <v>0</v>
       </c>
       <c r="AM131">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="AN131">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="AO131">
+        <f t="shared" si="1"/>
+        <v>490</v>
       </c>
     </row>
     <row r="132" spans="1:41">
-      <c r="A132" s="1"/>
+      <c r="A132" s="1">
+        <v>44011.641377314816</v>
+      </c>
       <c r="B132">
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F132">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G132">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H132">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I132">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J132">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K132">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="L132">
         <v>0</v>
@@ -17598,16 +17696,16 @@
         <v>0</v>
       </c>
       <c r="O132">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P132">
         <v>0</v>
       </c>
       <c r="Q132">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="R132">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="S132">
         <v>0</v>
@@ -17631,19 +17729,19 @@
         <v>0</v>
       </c>
       <c r="Z132">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AA132">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB132">
         <v>0</v>
       </c>
       <c r="AC132">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AD132">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AE132">
         <v>0</v>
@@ -17652,7 +17750,7 @@
         <v>0</v>
       </c>
       <c r="AG132">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH132">
         <v>0</v>
@@ -17661,52 +17759,58 @@
         <v>0</v>
       </c>
       <c r="AJ132">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AK132">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AL132">
         <v>0</v>
       </c>
       <c r="AM132">
-        <v>0</v>
+        <v>395</v>
       </c>
       <c r="AN132">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="AO132">
+        <f t="shared" si="1"/>
+        <v>566</v>
       </c>
     </row>
     <row r="133" spans="1:41">
-      <c r="A133" s="1"/>
+      <c r="A133" s="1">
+        <v>44012.659953703704</v>
+      </c>
       <c r="B133">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G133">
         <v>0</v>
       </c>
       <c r="H133">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I133">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J133">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="K133">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L133">
         <v>0</v>
@@ -17715,16 +17819,16 @@
         <v>0</v>
       </c>
       <c r="N133">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O133">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="P133">
         <v>0</v>
       </c>
       <c r="Q133">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R133">
         <v>0</v>
@@ -17733,16 +17837,16 @@
         <v>0</v>
       </c>
       <c r="T133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U133">
         <v>0</v>
       </c>
       <c r="V133">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="W133">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X133">
         <v>0</v>
@@ -17760,13 +17864,13 @@
         <v>0</v>
       </c>
       <c r="AC133">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AD133">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AE133">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF133">
         <v>0</v>
@@ -17781,7 +17885,7 @@
         <v>0</v>
       </c>
       <c r="AJ133">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK133">
         <v>0</v>
@@ -17790,79 +17894,85 @@
         <v>0</v>
       </c>
       <c r="AM133">
-        <v>0</v>
+        <v>344</v>
       </c>
       <c r="AN133">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="AO133">
+        <f t="shared" si="1"/>
+        <v>561</v>
       </c>
     </row>
     <row r="134" spans="1:41">
-      <c r="A134" s="1"/>
+      <c r="A134" s="1">
+        <v>44013.662534722222</v>
+      </c>
       <c r="B134">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F134">
         <v>0</v>
       </c>
       <c r="G134">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H134">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I134">
         <v>0</v>
       </c>
       <c r="J134">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K134">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L134">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="M134">
         <v>0</v>
       </c>
       <c r="N134">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O134">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="P134">
         <v>0</v>
       </c>
       <c r="Q134">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="R134">
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="S134">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="T134">
         <v>0</v>
       </c>
       <c r="U134">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="V134">
         <v>0</v>
       </c>
       <c r="W134">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X134">
         <v>0</v>
@@ -17871,7 +17981,7 @@
         <v>0</v>
       </c>
       <c r="Z134">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA134">
         <v>0</v>
@@ -17883,10 +17993,10 @@
         <v>0</v>
       </c>
       <c r="AD134">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE134">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF134">
         <v>0</v>
@@ -17898,10 +18008,10 @@
         <v>0</v>
       </c>
       <c r="AI134">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ134">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AK134">
         <v>0</v>
@@ -17910,85 +18020,91 @@
         <v>0</v>
       </c>
       <c r="AM134">
-        <v>0</v>
+        <v>406</v>
       </c>
       <c r="AN134">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="AO134">
+        <f t="shared" si="1"/>
+        <v>790</v>
       </c>
     </row>
     <row r="135" spans="1:41">
-      <c r="A135" s="1"/>
+      <c r="A135" s="1">
+        <v>44014.661319444444</v>
+      </c>
       <c r="B135">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="D135">
         <v>0</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F135">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G135">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H135">
         <v>0</v>
       </c>
       <c r="I135">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J135">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="K135">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="L135">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="M135">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N135">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O135">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P135">
         <v>0</v>
       </c>
       <c r="Q135">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="R135">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="S135">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="T135">
         <v>0</v>
       </c>
       <c r="U135">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V135">
         <v>0</v>
       </c>
       <c r="W135">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="X135">
         <v>0</v>
       </c>
       <c r="Y135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z135">
         <v>0</v>
@@ -17997,10 +18113,10 @@
         <v>0</v>
       </c>
       <c r="AB135">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC135">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AD135">
         <v>0</v>
@@ -18030,43 +18146,49 @@
         <v>0</v>
       </c>
       <c r="AM135">
-        <v>0</v>
+        <v>649</v>
       </c>
       <c r="AN135">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="AO135">
+        <f t="shared" si="1"/>
+        <v>626</v>
       </c>
     </row>
     <row r="136" spans="1:41">
-      <c r="A136" s="1"/>
+      <c r="A136" s="1">
+        <v>44015.661307870374</v>
+      </c>
       <c r="B136">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E136">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F136">
         <v>0</v>
       </c>
       <c r="G136">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I136">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J136">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="K136">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="L136">
         <v>0</v>
@@ -18075,19 +18197,19 @@
         <v>0</v>
       </c>
       <c r="N136">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O136">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="P136">
         <v>0</v>
       </c>
       <c r="Q136">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="R136">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S136">
         <v>0</v>
@@ -18096,13 +18218,13 @@
         <v>0</v>
       </c>
       <c r="U136">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V136">
         <v>0</v>
       </c>
       <c r="W136">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="X136">
         <v>0</v>
@@ -18111,7 +18233,7 @@
         <v>0</v>
       </c>
       <c r="Z136">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AA136">
         <v>0</v>
@@ -18120,7 +18242,7 @@
         <v>0</v>
       </c>
       <c r="AC136">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AD136">
         <v>0</v>
@@ -18129,10 +18251,10 @@
         <v>0</v>
       </c>
       <c r="AF136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG136">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH136">
         <v>0</v>
@@ -18150,28 +18272,34 @@
         <v>0</v>
       </c>
       <c r="AM136">
-        <v>0</v>
+        <v>268</v>
       </c>
       <c r="AN136">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AO136">
+        <f t="shared" si="1"/>
+        <v>454</v>
       </c>
     </row>
     <row r="137" spans="1:41">
-      <c r="A137" s="1"/>
+      <c r="A137" s="1">
+        <v>44016.649699074071</v>
+      </c>
       <c r="B137">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G137">
         <v>0</v>
@@ -18180,13 +18308,13 @@
         <v>0</v>
       </c>
       <c r="I137">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J137">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="K137">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L137">
         <v>0</v>
@@ -18198,37 +18326,37 @@
         <v>0</v>
       </c>
       <c r="O137">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P137">
         <v>0</v>
       </c>
       <c r="Q137">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R137">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="S137">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="T137">
         <v>0</v>
       </c>
       <c r="U137">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V137">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X137">
         <v>0</v>
       </c>
       <c r="Y137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z137">
         <v>0</v>
@@ -18240,19 +18368,19 @@
         <v>0</v>
       </c>
       <c r="AC137">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AD137">
         <v>0</v>
       </c>
       <c r="AE137">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF137">
         <v>0</v>
       </c>
       <c r="AG137">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH137">
         <v>0</v>
@@ -18270,67 +18398,73 @@
         <v>0</v>
       </c>
       <c r="AM137">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="AN137">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="AO137">
+        <f t="shared" si="1"/>
+        <v>603</v>
       </c>
     </row>
     <row r="138" spans="1:41">
-      <c r="A138" s="1"/>
+      <c r="A138" s="1">
+        <v>44017.650497685187</v>
+      </c>
       <c r="B138">
-        <v>0</v>
+        <v>199</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F138">
         <v>0</v>
       </c>
       <c r="G138">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H138">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I138">
         <v>0</v>
       </c>
       <c r="J138">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K138">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="L138">
         <v>0</v>
       </c>
       <c r="M138">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N138">
         <v>0</v>
       </c>
       <c r="O138">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q138">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="R138">
         <v>0</v>
       </c>
       <c r="S138">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T138">
         <v>0</v>
@@ -18342,7 +18476,7 @@
         <v>0</v>
       </c>
       <c r="W138">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X138">
         <v>0</v>
@@ -18357,10 +18491,10 @@
         <v>0</v>
       </c>
       <c r="AB138">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC138">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD138">
         <v>0</v>
@@ -18375,61 +18509,67 @@
         <v>0</v>
       </c>
       <c r="AH138">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI138">
         <v>0</v>
       </c>
       <c r="AJ138">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AK138">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="AL138">
         <v>0</v>
       </c>
       <c r="AM138">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="AN138">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="AO138">
+        <f t="shared" si="1"/>
+        <v>544</v>
       </c>
     </row>
     <row r="139" spans="1:41">
-      <c r="A139" s="1"/>
+      <c r="A139" s="1">
+        <v>44018.64875</v>
+      </c>
       <c r="B139">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D139">
         <v>0</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="F139">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G139">
         <v>0</v>
       </c>
       <c r="H139">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I139">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J139">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="K139">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="L139">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M139">
         <v>0</v>
@@ -18438,31 +18578,31 @@
         <v>0</v>
       </c>
       <c r="O139">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q139">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R139">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="S139">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="T139">
         <v>0</v>
       </c>
       <c r="U139">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V139">
         <v>0</v>
       </c>
       <c r="W139">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X139">
         <v>0</v>
@@ -18480,7 +18620,7 @@
         <v>0</v>
       </c>
       <c r="AC139">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AD139">
         <v>0</v>
@@ -18492,7 +18632,7 @@
         <v>0</v>
       </c>
       <c r="AG139">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH139">
         <v>0</v>
@@ -18501,55 +18641,61 @@
         <v>0</v>
       </c>
       <c r="AJ139">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AK139">
         <v>0</v>
       </c>
       <c r="AL139">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM139">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="AN139">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="AO139">
+        <f t="shared" si="1"/>
+        <v>575</v>
       </c>
     </row>
     <row r="140" spans="1:41">
-      <c r="A140" s="1"/>
+      <c r="A140" s="1">
+        <v>44019.6483912037</v>
+      </c>
       <c r="B140">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E140">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F140">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H140">
         <v>0</v>
       </c>
       <c r="I140">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J140">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="K140">
         <v>0</v>
       </c>
       <c r="L140">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M140">
         <v>0</v>
@@ -18558,31 +18704,31 @@
         <v>0</v>
       </c>
       <c r="O140">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P140">
         <v>0</v>
       </c>
       <c r="Q140">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="R140">
         <v>0</v>
       </c>
       <c r="S140">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T140">
         <v>0</v>
       </c>
       <c r="U140">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="V140">
         <v>0</v>
       </c>
       <c r="W140">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="X140">
         <v>0</v>
@@ -18591,7 +18737,7 @@
         <v>0</v>
       </c>
       <c r="Z140">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AA140">
         <v>0</v>
@@ -18600,28 +18746,28 @@
         <v>0</v>
       </c>
       <c r="AC140">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD140">
         <v>0</v>
       </c>
       <c r="AE140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF140">
         <v>0</v>
       </c>
       <c r="AG140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH140">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI140">
         <v>0</v>
       </c>
       <c r="AJ140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK140">
         <v>0</v>
@@ -18630,54 +18776,61 @@
         <v>0</v>
       </c>
       <c r="AM140">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="AN140">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="AO140">
+        <f t="shared" si="1"/>
+        <v>503</v>
       </c>
     </row>
     <row r="141" spans="1:41">
+      <c r="A141" s="1">
+        <v>44020.661886574075</v>
+      </c>
       <c r="B141">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F141">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H141">
         <v>0</v>
       </c>
       <c r="I141">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J141">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K141">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="L141">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M141">
         <v>0</v>
       </c>
       <c r="N141">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O141">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P141">
         <v>0</v>
@@ -18686,19 +18839,19 @@
         <v>0</v>
       </c>
       <c r="R141">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="S141">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="T141">
         <v>0</v>
       </c>
       <c r="U141">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="V141">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W141">
         <v>0</v>
@@ -18713,16 +18866,16 @@
         <v>0</v>
       </c>
       <c r="AA141">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC141">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AD141">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AE141">
         <v>0</v>
@@ -18740,7 +18893,7 @@
         <v>0</v>
       </c>
       <c r="AJ141">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AK141">
         <v>0</v>
@@ -18749,174 +18902,1419 @@
         <v>0</v>
       </c>
       <c r="AM141">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="AN141">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="AO141">
+        <f t="shared" si="1"/>
+        <v>460</v>
       </c>
     </row>
     <row r="142" spans="1:41">
+      <c r="A142" s="1">
+        <v>44021.646481481483</v>
+      </c>
       <c r="B142">
-        <f>SUM(B2:B141)</f>
-        <v>9741</v>
+        <v>157</v>
       </c>
       <c r="C142">
-        <f t="shared" ref="C142:AN142" si="2">SUM(C2:C141)</f>
-        <v>1676</v>
+        <v>17</v>
       </c>
       <c r="D142">
+        <v>11</v>
+      </c>
+      <c r="E142">
+        <v>6</v>
+      </c>
+      <c r="F142">
+        <v>2</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>18</v>
+      </c>
+      <c r="I142">
+        <v>21</v>
+      </c>
+      <c r="J142">
+        <v>59</v>
+      </c>
+      <c r="K142">
+        <v>31</v>
+      </c>
+      <c r="L142">
+        <v>4</v>
+      </c>
+      <c r="M142">
+        <v>22</v>
+      </c>
+      <c r="N142">
+        <v>0</v>
+      </c>
+      <c r="O142">
+        <v>18</v>
+      </c>
+      <c r="P142">
+        <v>1</v>
+      </c>
+      <c r="Q142">
+        <v>56</v>
+      </c>
+      <c r="R142">
+        <v>14</v>
+      </c>
+      <c r="S142">
+        <v>10</v>
+      </c>
+      <c r="T142">
+        <v>0</v>
+      </c>
+      <c r="U142">
+        <v>8</v>
+      </c>
+      <c r="V142">
+        <v>1</v>
+      </c>
+      <c r="W142">
+        <v>1</v>
+      </c>
+      <c r="X142">
+        <v>0</v>
+      </c>
+      <c r="Y142">
+        <v>0</v>
+      </c>
+      <c r="Z142">
+        <v>0</v>
+      </c>
+      <c r="AA142">
+        <v>0</v>
+      </c>
+      <c r="AB142">
+        <v>0</v>
+      </c>
+      <c r="AC142">
+        <v>19</v>
+      </c>
+      <c r="AD142">
+        <v>3</v>
+      </c>
+      <c r="AE142">
+        <v>0</v>
+      </c>
+      <c r="AF142">
+        <v>0</v>
+      </c>
+      <c r="AG142">
+        <v>2</v>
+      </c>
+      <c r="AH142">
+        <v>0</v>
+      </c>
+      <c r="AI142">
+        <v>1</v>
+      </c>
+      <c r="AJ142">
+        <v>17</v>
+      </c>
+      <c r="AK142">
+        <v>0</v>
+      </c>
+      <c r="AL142">
+        <v>0</v>
+      </c>
+      <c r="AM142">
+        <v>173</v>
+      </c>
+      <c r="AN142">
+        <v>5</v>
+      </c>
+      <c r="AO142">
+        <f t="shared" si="1"/>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="143" spans="1:41">
+      <c r="A143" s="1">
+        <v>44022.65519675926</v>
+      </c>
+      <c r="B143">
+        <v>224</v>
+      </c>
+      <c r="C143">
+        <v>68</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>3</v>
+      </c>
+      <c r="H143">
+        <v>9</v>
+      </c>
+      <c r="I143">
+        <v>2</v>
+      </c>
+      <c r="J143">
+        <v>31</v>
+      </c>
+      <c r="K143">
+        <v>85</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+      <c r="M143">
+        <v>0</v>
+      </c>
+      <c r="N143">
+        <v>0</v>
+      </c>
+      <c r="O143">
+        <v>39</v>
+      </c>
+      <c r="P143">
+        <v>0</v>
+      </c>
+      <c r="Q143">
+        <v>0</v>
+      </c>
+      <c r="R143">
+        <v>11</v>
+      </c>
+      <c r="S143">
+        <v>49</v>
+      </c>
+      <c r="T143">
+        <v>3</v>
+      </c>
+      <c r="U143">
+        <v>30</v>
+      </c>
+      <c r="V143">
+        <v>10</v>
+      </c>
+      <c r="W143">
+        <v>1</v>
+      </c>
+      <c r="X143">
+        <v>0</v>
+      </c>
+      <c r="Y143">
+        <v>0</v>
+      </c>
+      <c r="Z143">
+        <v>0</v>
+      </c>
+      <c r="AA143">
+        <v>0</v>
+      </c>
+      <c r="AB143">
+        <v>0</v>
+      </c>
+      <c r="AC143">
+        <v>2</v>
+      </c>
+      <c r="AD143">
+        <v>0</v>
+      </c>
+      <c r="AE143">
+        <v>0</v>
+      </c>
+      <c r="AF143">
+        <v>0</v>
+      </c>
+      <c r="AG143">
+        <v>2</v>
+      </c>
+      <c r="AH143">
+        <v>0</v>
+      </c>
+      <c r="AI143">
+        <v>0</v>
+      </c>
+      <c r="AJ143">
+        <v>0</v>
+      </c>
+      <c r="AK143">
+        <v>5</v>
+      </c>
+      <c r="AL143">
+        <v>0</v>
+      </c>
+      <c r="AM143">
+        <v>249</v>
+      </c>
+      <c r="AN143">
+        <v>20</v>
+      </c>
+      <c r="AO143">
+        <f t="shared" si="1"/>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="144" spans="1:41">
+      <c r="A144" s="1">
+        <v>44023.657442129632</v>
+      </c>
+      <c r="B144">
+        <v>224</v>
+      </c>
+      <c r="C144">
+        <v>105</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>17</v>
+      </c>
+      <c r="F144">
+        <v>19</v>
+      </c>
+      <c r="G144">
+        <v>3</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>85</v>
+      </c>
+      <c r="K144">
+        <v>17</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+      <c r="M144">
+        <v>0</v>
+      </c>
+      <c r="N144">
+        <v>0</v>
+      </c>
+      <c r="O144">
+        <v>32</v>
+      </c>
+      <c r="P144">
+        <v>3</v>
+      </c>
+      <c r="Q144">
+        <v>64</v>
+      </c>
+      <c r="R144">
+        <v>11</v>
+      </c>
+      <c r="S144">
+        <v>14</v>
+      </c>
+      <c r="T144">
+        <v>0</v>
+      </c>
+      <c r="U144">
+        <v>7</v>
+      </c>
+      <c r="V144">
+        <v>0</v>
+      </c>
+      <c r="W144">
+        <v>3</v>
+      </c>
+      <c r="X144">
+        <v>0</v>
+      </c>
+      <c r="Y144">
+        <v>0</v>
+      </c>
+      <c r="Z144">
+        <v>0</v>
+      </c>
+      <c r="AA144">
+        <v>0</v>
+      </c>
+      <c r="AB144">
+        <v>10</v>
+      </c>
+      <c r="AC144">
+        <v>17</v>
+      </c>
+      <c r="AD144">
+        <v>27</v>
+      </c>
+      <c r="AE144">
+        <v>0</v>
+      </c>
+      <c r="AF144">
+        <v>0</v>
+      </c>
+      <c r="AG144">
+        <v>6</v>
+      </c>
+      <c r="AH144">
+        <v>0</v>
+      </c>
+      <c r="AI144">
+        <v>0</v>
+      </c>
+      <c r="AJ144">
+        <v>0</v>
+      </c>
+      <c r="AK144">
+        <v>0</v>
+      </c>
+      <c r="AL144">
+        <v>0</v>
+      </c>
+      <c r="AM144">
+        <v>308</v>
+      </c>
+      <c r="AN144">
+        <v>15</v>
+      </c>
+      <c r="AO144">
+        <f t="shared" si="1"/>
+        <v>664</v>
+      </c>
+    </row>
+    <row r="145" spans="1:42">
+      <c r="A145" s="1">
+        <v>44024.639641203707</v>
+      </c>
+      <c r="B145">
+        <v>152</v>
+      </c>
+      <c r="C145">
+        <v>38</v>
+      </c>
+      <c r="D145">
+        <v>6</v>
+      </c>
+      <c r="E145">
+        <v>7</v>
+      </c>
+      <c r="F145">
+        <v>14</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>14</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>53</v>
+      </c>
+      <c r="K145">
+        <v>20</v>
+      </c>
+      <c r="L145">
+        <v>19</v>
+      </c>
+      <c r="M145">
+        <v>11</v>
+      </c>
+      <c r="N145">
+        <v>2</v>
+      </c>
+      <c r="O145">
+        <v>11</v>
+      </c>
+      <c r="P145">
+        <v>14</v>
+      </c>
+      <c r="Q145">
+        <v>46</v>
+      </c>
+      <c r="R145">
+        <v>0</v>
+      </c>
+      <c r="S145">
+        <v>11</v>
+      </c>
+      <c r="T145">
+        <v>0</v>
+      </c>
+      <c r="U145">
+        <v>0</v>
+      </c>
+      <c r="V145">
+        <v>10</v>
+      </c>
+      <c r="W145">
+        <v>0</v>
+      </c>
+      <c r="X145">
+        <v>0</v>
+      </c>
+      <c r="Y145">
+        <v>0</v>
+      </c>
+      <c r="Z145">
+        <v>0</v>
+      </c>
+      <c r="AA145">
+        <v>0</v>
+      </c>
+      <c r="AB145">
+        <v>0</v>
+      </c>
+      <c r="AC145">
+        <v>17</v>
+      </c>
+      <c r="AD145">
+        <v>0</v>
+      </c>
+      <c r="AE145">
+        <v>0</v>
+      </c>
+      <c r="AF145">
+        <v>0</v>
+      </c>
+      <c r="AG145">
+        <v>0</v>
+      </c>
+      <c r="AH145">
+        <v>0</v>
+      </c>
+      <c r="AI145">
+        <v>0</v>
+      </c>
+      <c r="AJ145">
+        <v>14</v>
+      </c>
+      <c r="AK145">
+        <v>108</v>
+      </c>
+      <c r="AL145">
+        <v>4</v>
+      </c>
+      <c r="AM145">
+        <v>344</v>
+      </c>
+      <c r="AN145">
+        <v>16</v>
+      </c>
+      <c r="AO145">
+        <f t="shared" si="1"/>
+        <v>571</v>
+      </c>
+    </row>
+    <row r="146" spans="1:42">
+      <c r="A146" s="1">
+        <v>44025.65216435185</v>
+      </c>
+      <c r="B146">
+        <v>156</v>
+      </c>
+      <c r="C146">
+        <v>99</v>
+      </c>
+      <c r="D146">
+        <v>5</v>
+      </c>
+      <c r="E146">
+        <v>4</v>
+      </c>
+      <c r="F146">
+        <v>17</v>
+      </c>
+      <c r="G146">
+        <v>3</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>5</v>
+      </c>
+      <c r="J146">
+        <v>47</v>
+      </c>
+      <c r="K146">
+        <v>141</v>
+      </c>
+      <c r="L146">
+        <v>0</v>
+      </c>
+      <c r="M146">
+        <v>0</v>
+      </c>
+      <c r="N146">
+        <v>0</v>
+      </c>
+      <c r="O146">
+        <v>27</v>
+      </c>
+      <c r="P146">
+        <v>0</v>
+      </c>
+      <c r="Q146">
+        <v>22</v>
+      </c>
+      <c r="R146">
+        <v>0</v>
+      </c>
+      <c r="S146">
+        <v>20</v>
+      </c>
+      <c r="T146">
+        <v>0</v>
+      </c>
+      <c r="U146">
+        <v>0</v>
+      </c>
+      <c r="V146">
+        <v>0</v>
+      </c>
+      <c r="W146">
+        <v>0</v>
+      </c>
+      <c r="X146">
+        <v>0</v>
+      </c>
+      <c r="Y146">
+        <v>0</v>
+      </c>
+      <c r="Z146">
+        <v>5</v>
+      </c>
+      <c r="AA146">
+        <v>8</v>
+      </c>
+      <c r="AB146">
+        <v>0</v>
+      </c>
+      <c r="AC146">
+        <v>10</v>
+      </c>
+      <c r="AD146">
+        <v>13</v>
+      </c>
+      <c r="AE146">
+        <v>1</v>
+      </c>
+      <c r="AF146">
+        <v>0</v>
+      </c>
+      <c r="AG146">
+        <v>8</v>
+      </c>
+      <c r="AH146">
+        <v>3</v>
+      </c>
+      <c r="AI146">
+        <v>0</v>
+      </c>
+      <c r="AJ146">
+        <v>0</v>
+      </c>
+      <c r="AK146">
+        <v>0</v>
+      </c>
+      <c r="AL146">
+        <v>1</v>
+      </c>
+      <c r="AM146">
+        <v>224</v>
+      </c>
+      <c r="AN146">
+        <v>4</v>
+      </c>
+      <c r="AO146">
+        <f t="shared" si="1"/>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="147" spans="1:42">
+      <c r="A147" s="1">
+        <v>44026.651354166665</v>
+      </c>
+      <c r="B147">
+        <v>128</v>
+      </c>
+      <c r="C147">
+        <v>12</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>14</v>
+      </c>
+      <c r="F147">
+        <v>14</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="I147">
+        <v>2</v>
+      </c>
+      <c r="J147">
+        <v>29</v>
+      </c>
+      <c r="K147">
+        <v>15</v>
+      </c>
+      <c r="L147">
+        <v>92</v>
+      </c>
+      <c r="M147">
+        <v>0</v>
+      </c>
+      <c r="N147">
+        <v>0</v>
+      </c>
+      <c r="O147">
+        <v>23</v>
+      </c>
+      <c r="P147">
+        <v>3</v>
+      </c>
+      <c r="Q147">
+        <v>9</v>
+      </c>
+      <c r="R147">
+        <v>33</v>
+      </c>
+      <c r="S147">
+        <v>9</v>
+      </c>
+      <c r="T147">
+        <v>0</v>
+      </c>
+      <c r="U147">
+        <v>39</v>
+      </c>
+      <c r="V147">
+        <v>0</v>
+      </c>
+      <c r="W147">
+        <v>8</v>
+      </c>
+      <c r="X147">
+        <v>0</v>
+      </c>
+      <c r="Y147">
+        <v>0</v>
+      </c>
+      <c r="Z147">
+        <v>0</v>
+      </c>
+      <c r="AA147">
+        <v>0</v>
+      </c>
+      <c r="AB147">
+        <v>0</v>
+      </c>
+      <c r="AC147">
+        <v>28</v>
+      </c>
+      <c r="AD147">
+        <v>0</v>
+      </c>
+      <c r="AE147">
+        <v>0</v>
+      </c>
+      <c r="AF147">
+        <v>0</v>
+      </c>
+      <c r="AG147">
+        <v>0</v>
+      </c>
+      <c r="AH147">
+        <v>0</v>
+      </c>
+      <c r="AI147">
+        <v>0</v>
+      </c>
+      <c r="AJ147">
+        <v>5</v>
+      </c>
+      <c r="AK147">
+        <v>0</v>
+      </c>
+      <c r="AL147">
+        <v>0</v>
+      </c>
+      <c r="AM147">
+        <v>121</v>
+      </c>
+      <c r="AN147">
+        <v>10</v>
+      </c>
+      <c r="AO147">
+        <f t="shared" si="1"/>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="148" spans="1:42">
+      <c r="A148" s="1">
+        <v>44027.705127314817</v>
+      </c>
+      <c r="B148">
+        <v>230</v>
+      </c>
+      <c r="C148">
+        <v>51</v>
+      </c>
+      <c r="D148">
+        <v>4</v>
+      </c>
+      <c r="E148">
+        <v>27</v>
+      </c>
+      <c r="F148">
+        <v>35</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>0</v>
+      </c>
+      <c r="J148">
+        <v>43</v>
+      </c>
+      <c r="K148">
+        <v>69</v>
+      </c>
+      <c r="L148">
+        <v>0</v>
+      </c>
+      <c r="M148">
+        <v>0</v>
+      </c>
+      <c r="N148">
+        <v>0</v>
+      </c>
+      <c r="O148">
+        <v>28</v>
+      </c>
+      <c r="P148">
+        <v>1</v>
+      </c>
+      <c r="Q148">
+        <v>23</v>
+      </c>
+      <c r="R148">
+        <v>6</v>
+      </c>
+      <c r="S148">
+        <v>30</v>
+      </c>
+      <c r="T148">
+        <v>0</v>
+      </c>
+      <c r="U148">
+        <v>16</v>
+      </c>
+      <c r="V148">
+        <v>0</v>
+      </c>
+      <c r="W148">
+        <v>0</v>
+      </c>
+      <c r="X148">
+        <v>0</v>
+      </c>
+      <c r="Y148">
+        <v>0</v>
+      </c>
+      <c r="Z148">
+        <v>17</v>
+      </c>
+      <c r="AA148">
+        <v>0</v>
+      </c>
+      <c r="AB148">
+        <v>0</v>
+      </c>
+      <c r="AC148">
+        <v>20</v>
+      </c>
+      <c r="AD148">
+        <v>10</v>
+      </c>
+      <c r="AE148">
+        <v>1</v>
+      </c>
+      <c r="AF148">
+        <v>0</v>
+      </c>
+      <c r="AG148">
+        <v>2</v>
+      </c>
+      <c r="AH148">
+        <v>0</v>
+      </c>
+      <c r="AI148">
+        <v>0</v>
+      </c>
+      <c r="AJ148">
+        <v>0</v>
+      </c>
+      <c r="AK148">
+        <v>30</v>
+      </c>
+      <c r="AL148">
+        <v>0</v>
+      </c>
+      <c r="AM148">
+        <v>207</v>
+      </c>
+      <c r="AN148">
+        <v>6</v>
+      </c>
+      <c r="AO148">
+        <f t="shared" si="1"/>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="149" spans="1:42">
+      <c r="A149" s="1"/>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
+      <c r="L149">
+        <v>0</v>
+      </c>
+      <c r="M149">
+        <v>0</v>
+      </c>
+      <c r="N149">
+        <v>0</v>
+      </c>
+      <c r="O149">
+        <v>0</v>
+      </c>
+      <c r="P149">
+        <v>0</v>
+      </c>
+      <c r="Q149">
+        <v>0</v>
+      </c>
+      <c r="R149">
+        <v>0</v>
+      </c>
+      <c r="S149">
+        <v>0</v>
+      </c>
+      <c r="T149">
+        <v>0</v>
+      </c>
+      <c r="U149">
+        <v>0</v>
+      </c>
+      <c r="V149">
+        <v>0</v>
+      </c>
+      <c r="W149">
+        <v>0</v>
+      </c>
+      <c r="X149">
+        <v>0</v>
+      </c>
+      <c r="Y149">
+        <v>0</v>
+      </c>
+      <c r="Z149">
+        <v>0</v>
+      </c>
+      <c r="AA149">
+        <v>0</v>
+      </c>
+      <c r="AB149">
+        <v>0</v>
+      </c>
+      <c r="AC149">
+        <v>0</v>
+      </c>
+      <c r="AD149">
+        <v>0</v>
+      </c>
+      <c r="AE149">
+        <v>0</v>
+      </c>
+      <c r="AF149">
+        <v>0</v>
+      </c>
+      <c r="AG149">
+        <v>0</v>
+      </c>
+      <c r="AH149">
+        <v>0</v>
+      </c>
+      <c r="AI149">
+        <v>0</v>
+      </c>
+      <c r="AJ149">
+        <v>0</v>
+      </c>
+      <c r="AK149">
+        <v>0</v>
+      </c>
+      <c r="AL149">
+        <v>0</v>
+      </c>
+      <c r="AM149">
+        <v>0</v>
+      </c>
+      <c r="AN149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:42">
+      <c r="A150" s="1"/>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>0</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150">
+        <v>0</v>
+      </c>
+      <c r="L150">
+        <v>0</v>
+      </c>
+      <c r="M150">
+        <v>0</v>
+      </c>
+      <c r="N150">
+        <v>0</v>
+      </c>
+      <c r="O150">
+        <v>0</v>
+      </c>
+      <c r="P150">
+        <v>0</v>
+      </c>
+      <c r="Q150">
+        <v>0</v>
+      </c>
+      <c r="R150">
+        <v>0</v>
+      </c>
+      <c r="S150">
+        <v>0</v>
+      </c>
+      <c r="T150">
+        <v>0</v>
+      </c>
+      <c r="U150">
+        <v>0</v>
+      </c>
+      <c r="V150">
+        <v>0</v>
+      </c>
+      <c r="W150">
+        <v>0</v>
+      </c>
+      <c r="X150">
+        <v>0</v>
+      </c>
+      <c r="Y150">
+        <v>0</v>
+      </c>
+      <c r="Z150">
+        <v>0</v>
+      </c>
+      <c r="AA150">
+        <v>0</v>
+      </c>
+      <c r="AB150">
+        <v>0</v>
+      </c>
+      <c r="AC150">
+        <v>0</v>
+      </c>
+      <c r="AD150">
+        <v>0</v>
+      </c>
+      <c r="AE150">
+        <v>0</v>
+      </c>
+      <c r="AF150">
+        <v>0</v>
+      </c>
+      <c r="AG150">
+        <v>0</v>
+      </c>
+      <c r="AH150">
+        <v>0</v>
+      </c>
+      <c r="AI150">
+        <v>0</v>
+      </c>
+      <c r="AJ150">
+        <v>0</v>
+      </c>
+      <c r="AK150">
+        <v>0</v>
+      </c>
+      <c r="AL150">
+        <v>0</v>
+      </c>
+      <c r="AM150">
+        <v>0</v>
+      </c>
+      <c r="AN150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:42">
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+      <c r="K151">
+        <v>0</v>
+      </c>
+      <c r="L151">
+        <v>0</v>
+      </c>
+      <c r="M151">
+        <v>0</v>
+      </c>
+      <c r="N151">
+        <v>0</v>
+      </c>
+      <c r="O151">
+        <v>0</v>
+      </c>
+      <c r="P151">
+        <v>0</v>
+      </c>
+      <c r="Q151">
+        <v>0</v>
+      </c>
+      <c r="R151">
+        <v>0</v>
+      </c>
+      <c r="S151">
+        <v>0</v>
+      </c>
+      <c r="T151">
+        <v>0</v>
+      </c>
+      <c r="U151">
+        <v>0</v>
+      </c>
+      <c r="V151">
+        <v>0</v>
+      </c>
+      <c r="W151">
+        <v>0</v>
+      </c>
+      <c r="X151">
+        <v>0</v>
+      </c>
+      <c r="Y151">
+        <v>0</v>
+      </c>
+      <c r="Z151">
+        <v>0</v>
+      </c>
+      <c r="AA151">
+        <v>0</v>
+      </c>
+      <c r="AB151">
+        <v>0</v>
+      </c>
+      <c r="AC151">
+        <v>0</v>
+      </c>
+      <c r="AD151">
+        <v>0</v>
+      </c>
+      <c r="AE151">
+        <v>0</v>
+      </c>
+      <c r="AF151">
+        <v>0</v>
+      </c>
+      <c r="AG151">
+        <v>0</v>
+      </c>
+      <c r="AH151">
+        <v>0</v>
+      </c>
+      <c r="AI151">
+        <v>0</v>
+      </c>
+      <c r="AJ151">
+        <v>0</v>
+      </c>
+      <c r="AK151">
+        <v>0</v>
+      </c>
+      <c r="AL151">
+        <v>0</v>
+      </c>
+      <c r="AM151">
+        <v>0</v>
+      </c>
+      <c r="AN151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:42">
+      <c r="B152">
+        <f>SUM(B2:B151)</f>
+        <v>12941</v>
+      </c>
+      <c r="C152">
+        <f t="shared" ref="C152:AN152" si="2">SUM(C2:C151)</f>
+        <v>2738</v>
+      </c>
+      <c r="D152">
         <f t="shared" si="2"/>
-        <v>1191</v>
-      </c>
-      <c r="E142">
+        <v>1318</v>
+      </c>
+      <c r="E152">
         <f t="shared" si="2"/>
-        <v>756</v>
-      </c>
-      <c r="F142">
+        <v>1132</v>
+      </c>
+      <c r="F152">
         <f t="shared" si="2"/>
-        <v>106</v>
-      </c>
-      <c r="G142">
+        <v>311</v>
+      </c>
+      <c r="G152">
         <f t="shared" si="2"/>
-        <v>487</v>
-      </c>
-      <c r="H142">
+        <v>533</v>
+      </c>
+      <c r="H152">
         <f t="shared" si="2"/>
-        <v>528</v>
-      </c>
-      <c r="I142">
+        <v>669</v>
+      </c>
+      <c r="I152">
         <f t="shared" si="2"/>
-        <v>477</v>
-      </c>
-      <c r="J142">
+        <v>593</v>
+      </c>
+      <c r="J152">
         <f t="shared" si="2"/>
-        <v>873</v>
-      </c>
-      <c r="K142">
+        <v>1850</v>
+      </c>
+      <c r="K152">
         <f t="shared" si="2"/>
-        <v>1264</v>
-      </c>
-      <c r="L142">
+        <v>1951</v>
+      </c>
+      <c r="L152">
         <f t="shared" si="2"/>
-        <v>217</v>
-      </c>
-      <c r="M142">
+        <v>422</v>
+      </c>
+      <c r="M152">
         <f t="shared" si="2"/>
-        <v>83</v>
-      </c>
-      <c r="N142">
+        <v>145</v>
+      </c>
+      <c r="N152">
         <f t="shared" si="2"/>
-        <v>497</v>
-      </c>
-      <c r="O142">
+        <v>521</v>
+      </c>
+      <c r="O152">
         <f t="shared" si="2"/>
-        <v>684</v>
-      </c>
-      <c r="P142">
+        <v>1067</v>
+      </c>
+      <c r="P152">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="Q142">
+        <v>67</v>
+      </c>
+      <c r="Q152">
         <f t="shared" si="2"/>
-        <v>216</v>
-      </c>
-      <c r="R142">
+        <v>770</v>
+      </c>
+      <c r="R152">
         <f t="shared" si="2"/>
-        <v>781</v>
-      </c>
-      <c r="S142">
+        <v>1398</v>
+      </c>
+      <c r="S152">
         <f t="shared" si="2"/>
-        <v>982</v>
-      </c>
-      <c r="T142">
+        <v>1427</v>
+      </c>
+      <c r="T152">
         <f t="shared" si="2"/>
-        <v>317</v>
-      </c>
-      <c r="U142">
+        <v>321</v>
+      </c>
+      <c r="U152">
         <f t="shared" si="2"/>
-        <v>202</v>
-      </c>
-      <c r="V142">
+        <v>531</v>
+      </c>
+      <c r="V152">
         <f t="shared" si="2"/>
-        <v>84</v>
-      </c>
-      <c r="W142">
+        <v>145</v>
+      </c>
+      <c r="W152">
         <f t="shared" si="2"/>
-        <v>297</v>
-      </c>
-      <c r="X142">
+        <v>413</v>
+      </c>
+      <c r="X152">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="Y142">
+      <c r="Y152">
         <f t="shared" si="2"/>
-        <v>141</v>
-      </c>
-      <c r="Z142">
+        <v>154</v>
+      </c>
+      <c r="Z152">
         <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="AA142">
+        <v>143</v>
+      </c>
+      <c r="AA152">
         <f t="shared" si="2"/>
-        <v>71</v>
-      </c>
-      <c r="AB142">
+        <v>101</v>
+      </c>
+      <c r="AB152">
         <f t="shared" si="2"/>
-        <v>73</v>
-      </c>
-      <c r="AC142">
+        <v>110</v>
+      </c>
+      <c r="AC152">
         <f t="shared" si="2"/>
-        <v>298</v>
-      </c>
-      <c r="AD142">
+        <v>591</v>
+      </c>
+      <c r="AD152">
         <f t="shared" si="2"/>
-        <v>278</v>
-      </c>
-      <c r="AE142">
+        <v>409</v>
+      </c>
+      <c r="AE152">
         <f t="shared" si="2"/>
-        <v>71</v>
-      </c>
-      <c r="AF142">
+        <v>88</v>
+      </c>
+      <c r="AF152">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="AG142">
+        <v>5</v>
+      </c>
+      <c r="AG152">
         <f t="shared" si="2"/>
-        <v>198</v>
-      </c>
-      <c r="AH142">
+        <v>254</v>
+      </c>
+      <c r="AH152">
         <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="AI142">
+        <v>30</v>
+      </c>
+      <c r="AI152">
         <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-      <c r="AJ142">
+        <v>62</v>
+      </c>
+      <c r="AJ152">
         <f t="shared" si="2"/>
-        <v>184</v>
-      </c>
-      <c r="AK142">
+        <v>318</v>
+      </c>
+      <c r="AK152">
         <f t="shared" si="2"/>
-        <v>285</v>
-      </c>
-      <c r="AL142">
+        <v>646</v>
+      </c>
+      <c r="AL152">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM142">
+        <v>10</v>
+      </c>
+      <c r="AM152">
         <f t="shared" si="2"/>
-        <v>8253</v>
-      </c>
-      <c r="AN142">
+        <v>13999</v>
+      </c>
+      <c r="AN152">
         <f t="shared" si="2"/>
-        <v>554</v>
+        <v>760</v>
       </c>
     </row>
-    <row r="145" spans="42:42">
-      <c r="AP145">
-        <f>SUM(AO2:AO129)</f>
-        <v>23299</v>
+    <row r="155" spans="1:42">
+      <c r="AP155">
+        <f>SUM(AO2:AO148)</f>
+        <v>34260</v>
       </c>
     </row>
   </sheetData>
@@ -18933,11 +20331,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN129"/>
+  <dimension ref="A1:AO129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z131" sqref="Z131"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP9" sqref="AP9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18945,7 +20343,7 @@
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -19066,8 +20464,11 @@
       <c r="AN1" t="s">
         <v>37</v>
       </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:41">
       <c r="A2" s="1">
         <v>43888.653217592589</v>
       </c>
@@ -19188,8 +20589,11 @@
       <c r="AN2">
         <v>0</v>
       </c>
+      <c r="AO2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:41">
       <c r="A3" s="1">
         <v>43889.042083333334</v>
       </c>
@@ -19310,8 +20714,11 @@
       <c r="AN3">
         <v>0</v>
       </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:41">
       <c r="A4" s="1">
         <v>43890.101990740739</v>
       </c>
@@ -19432,8 +20839,11 @@
       <c r="AN4">
         <v>0</v>
       </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:41">
       <c r="A5" s="1">
         <v>43891.947314814817</v>
       </c>
@@ -19554,8 +20964,11 @@
       <c r="AN5">
         <v>0</v>
       </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:41">
       <c r="A6" s="1">
         <v>43892.495162037034</v>
       </c>
@@ -19676,8 +21089,11 @@
       <c r="AN6">
         <v>0</v>
       </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:41">
       <c r="A7" s="1">
         <v>43893.573935185188</v>
       </c>
@@ -19798,8 +21214,11 @@
       <c r="AN7">
         <v>0</v>
       </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:41">
       <c r="A8" s="1">
         <v>43894.98841435185</v>
       </c>
@@ -19920,8 +21339,11 @@
       <c r="AN8">
         <v>0</v>
       </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:41">
       <c r="A9" s="1">
         <v>43895.455000000002</v>
       </c>
@@ -20042,8 +21464,11 @@
       <c r="AN9">
         <v>0</v>
       </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:41">
       <c r="A10" s="1">
         <v>43896.191331018519</v>
       </c>
@@ -20164,8 +21589,11 @@
       <c r="AN10">
         <v>0</v>
       </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:41">
       <c r="A11" s="1">
         <v>43897.299085648148</v>
       </c>
@@ -20286,8 +21714,11 @@
       <c r="AN11">
         <v>0</v>
       </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:41">
       <c r="A12" s="1">
         <v>43898.433333333334</v>
       </c>
@@ -20408,8 +21839,11 @@
       <c r="AN12">
         <v>0</v>
       </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:41">
       <c r="A13" s="1">
         <v>43899.12159722222</v>
       </c>
@@ -20530,8 +21964,11 @@
       <c r="AN13">
         <v>0</v>
       </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:41">
       <c r="A14" s="1">
         <v>43900.040821759256</v>
       </c>
@@ -20652,8 +22089,11 @@
       <c r="AN14">
         <v>0</v>
       </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:41">
       <c r="A15" s="1">
         <v>43901.979224537034</v>
       </c>
@@ -20774,8 +22214,11 @@
       <c r="AN15">
         <v>0</v>
       </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:41">
       <c r="A16" s="1">
         <v>43902.444004629629</v>
       </c>
@@ -20896,8 +22339,11 @@
       <c r="AN16">
         <v>0</v>
       </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:41">
       <c r="A17" s="1">
         <v>43903.627766203703</v>
       </c>
@@ -21018,8 +22464,11 @@
       <c r="AN17">
         <v>0</v>
       </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:41">
       <c r="A18" s="1">
         <v>43904.682037037041</v>
       </c>
@@ -21140,8 +22589,11 @@
       <c r="AN18">
         <v>0</v>
       </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:41">
       <c r="A19" s="1">
         <v>43905.982592592591</v>
       </c>
@@ -21262,8 +22714,11 @@
       <c r="AN19">
         <v>0</v>
       </c>
+      <c r="AO19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:41">
       <c r="A20" s="1">
         <v>43906.245150462964</v>
       </c>
@@ -21384,8 +22839,11 @@
       <c r="AN20">
         <v>0</v>
       </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:41">
       <c r="A21" s="1">
         <v>43907.109988425924</v>
       </c>
@@ -21506,8 +22964,11 @@
       <c r="AN21">
         <v>0</v>
       </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:41">
       <c r="A22" s="1">
         <v>43908.359942129631</v>
       </c>
@@ -21628,8 +23089,11 @@
       <c r="AN22">
         <v>0</v>
       </c>
+      <c r="AO22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:41">
       <c r="A23" s="1">
         <v>43909.612037037034</v>
       </c>
@@ -21750,8 +23214,11 @@
       <c r="AN23">
         <v>0</v>
       </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:41">
       <c r="A24" s="1">
         <v>43910.305115740739</v>
       </c>
@@ -21872,8 +23339,11 @@
       <c r="AN24">
         <v>0</v>
       </c>
+      <c r="AO24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:41">
       <c r="A25" s="1">
         <v>43911.948449074072</v>
       </c>
@@ -21994,8 +23464,11 @@
       <c r="AN25">
         <v>0</v>
       </c>
+      <c r="AO25">
+        <v>3</v>
+      </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:41">
       <c r="A26" s="1">
         <v>43912.011678240742</v>
       </c>
@@ -22116,8 +23589,11 @@
       <c r="AN26">
         <v>0</v>
       </c>
+      <c r="AO26">
+        <v>21</v>
+      </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:41">
       <c r="A27" s="1">
         <v>43913.073622685188</v>
       </c>
@@ -22238,8 +23714,11 @@
       <c r="AN27">
         <v>1</v>
       </c>
+      <c r="AO27">
+        <v>12</v>
+      </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:41">
       <c r="A28" s="1">
         <v>43914.210648148146</v>
       </c>
@@ -22360,8 +23839,11 @@
       <c r="AN28">
         <v>0</v>
       </c>
+      <c r="AO28">
+        <v>4</v>
+      </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:41">
       <c r="A29" s="1">
         <v>43914.958784722221</v>
       </c>
@@ -22482,8 +23964,11 @@
       <c r="AN29">
         <v>0</v>
       </c>
+      <c r="AO29">
+        <v>2</v>
+      </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:41">
       <c r="A30" s="1">
         <v>43915.643657407411</v>
       </c>
@@ -22604,8 +24089,11 @@
       <c r="AN30">
         <v>0</v>
       </c>
+      <c r="AO30">
+        <v>5</v>
+      </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:41">
       <c r="A31" s="1">
         <v>43916.52484953704</v>
       </c>
@@ -22726,8 +24214,11 @@
       <c r="AN31">
         <v>0</v>
       </c>
+      <c r="AO31">
+        <v>14</v>
+      </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:41">
       <c r="A32" s="1">
         <v>43917.500486111108</v>
       </c>
@@ -22848,8 +24339,11 @@
       <c r="AN32">
         <v>0</v>
       </c>
+      <c r="AO32">
+        <v>5</v>
+      </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:41">
       <c r="A33" s="1">
         <v>43917.663784722223</v>
       </c>
@@ -22970,8 +24464,11 @@
       <c r="AN33">
         <v>0</v>
       </c>
+      <c r="AO33">
+        <v>11</v>
+      </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:41">
       <c r="A34" s="1">
         <v>43918.341932870368</v>
       </c>
@@ -23092,8 +24589,11 @@
       <c r="AN34">
         <v>0</v>
       </c>
+      <c r="AO34">
+        <v>8</v>
+      </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:41">
       <c r="A35" s="1">
         <v>43918.611828703702</v>
       </c>
@@ -23214,8 +24714,11 @@
       <c r="AN35">
         <v>0</v>
       </c>
+      <c r="AO35">
+        <v>8</v>
+      </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:41">
       <c r="A36" s="1">
         <v>43919.569398148145</v>
       </c>
@@ -23336,8 +24839,11 @@
       <c r="AN36">
         <v>0</v>
       </c>
+      <c r="AO36">
+        <v>14</v>
+      </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:41">
       <c r="A37" s="1">
         <v>43920.541979166665</v>
       </c>
@@ -23458,8 +24964,11 @@
       <c r="AN37">
         <v>1</v>
       </c>
+      <c r="AO37">
+        <v>20</v>
+      </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:41">
       <c r="A38" s="1">
         <v>43921.137361111112</v>
       </c>
@@ -23580,8 +25089,11 @@
       <c r="AN38">
         <v>0</v>
       </c>
+      <c r="AO38">
+        <v>4</v>
+      </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:41">
       <c r="A39" s="1">
         <v>43921.500358796293</v>
       </c>
@@ -23702,8 +25214,11 @@
       <c r="AN39">
         <v>0</v>
       </c>
+      <c r="AO39">
+        <v>4</v>
+      </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:41">
       <c r="A40" s="1">
         <v>43922.187604166669</v>
       </c>
@@ -23824,8 +25339,11 @@
       <c r="AN40">
         <v>0</v>
       </c>
+      <c r="AO40">
+        <v>12</v>
+      </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:41">
       <c r="A41" s="1">
         <v>43922.500208333331</v>
       </c>
@@ -23946,8 +25464,11 @@
       <c r="AN41">
         <v>0</v>
       </c>
+      <c r="AO41">
+        <v>23</v>
+      </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:41">
       <c r="A42" s="1">
         <v>43923.500648148147</v>
       </c>
@@ -24068,8 +25589,11 @@
       <c r="AN42">
         <v>0</v>
       </c>
+      <c r="AO42">
+        <v>10</v>
+      </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:41">
       <c r="A43" s="1">
         <v>43924.126400462963</v>
       </c>
@@ -24190,8 +25714,11 @@
       <c r="AN43">
         <v>0</v>
       </c>
+      <c r="AO43">
+        <v>6</v>
+      </c>
     </row>
-    <row r="44" spans="1:40">
+    <row r="44" spans="1:41">
       <c r="A44" s="1">
         <v>43925.590798611112</v>
       </c>
@@ -24312,8 +25839,11 @@
       <c r="AN44">
         <v>2</v>
       </c>
+      <c r="AO44">
+        <v>24</v>
+      </c>
     </row>
-    <row r="45" spans="1:40">
+    <row r="45" spans="1:41">
       <c r="A45" s="1">
         <v>43926.142210648148</v>
       </c>
@@ -24434,8 +25964,11 @@
       <c r="AN45">
         <v>1</v>
       </c>
+      <c r="AO45">
+        <v>10</v>
+      </c>
     </row>
-    <row r="46" spans="1:40">
+    <row r="46" spans="1:41">
       <c r="A46" s="1">
         <v>43926.564062500001</v>
       </c>
@@ -24556,8 +26089,11 @@
       <c r="AN46">
         <v>0</v>
       </c>
+      <c r="AO46">
+        <v>8</v>
+      </c>
     </row>
-    <row r="47" spans="1:40">
+    <row r="47" spans="1:41">
       <c r="A47" s="1">
         <v>43927.56287037037</v>
       </c>
@@ -24678,8 +26214,11 @@
       <c r="AN47">
         <v>0</v>
       </c>
+      <c r="AO47">
+        <v>6</v>
+      </c>
     </row>
-    <row r="48" spans="1:40">
+    <row r="48" spans="1:41">
       <c r="A48" s="1">
         <v>43928.563379629632</v>
       </c>
@@ -24800,8 +26339,11 @@
       <c r="AN48">
         <v>1</v>
       </c>
+      <c r="AO48">
+        <v>16</v>
+      </c>
     </row>
-    <row r="49" spans="1:40">
+    <row r="49" spans="1:41">
       <c r="A49" s="1">
         <v>43929.542685185188</v>
       </c>
@@ -24922,8 +26464,11 @@
       <c r="AN49">
         <v>0</v>
       </c>
+      <c r="AO49">
+        <v>22</v>
+      </c>
     </row>
-    <row r="50" spans="1:40">
+    <row r="50" spans="1:41">
       <c r="A50" s="1">
         <v>43930.563101851854</v>
       </c>
@@ -25044,8 +26589,11 @@
       <c r="AN50">
         <v>1</v>
       </c>
+      <c r="AO50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="51" spans="1:40">
+    <row r="51" spans="1:41">
       <c r="A51" s="1">
         <v>43931.568472222221</v>
       </c>
@@ -25166,8 +26714,11 @@
       <c r="AN51">
         <v>0</v>
       </c>
+      <c r="AO51">
+        <v>17</v>
+      </c>
     </row>
-    <row r="52" spans="1:40">
+    <row r="52" spans="1:41">
       <c r="A52" s="1">
         <v>43932.562881944446</v>
       </c>
@@ -25288,8 +26839,11 @@
       <c r="AN52">
         <v>3</v>
       </c>
+      <c r="AO52">
+        <v>13</v>
+      </c>
     </row>
-    <row r="53" spans="1:40">
+    <row r="53" spans="1:41">
       <c r="A53" s="1">
         <v>43933.549942129626</v>
       </c>
@@ -25410,8 +26964,11 @@
       <c r="AN53">
         <v>0</v>
       </c>
+      <c r="AO53">
+        <v>5</v>
+      </c>
     </row>
-    <row r="54" spans="1:40">
+    <row r="54" spans="1:41">
       <c r="A54" s="1">
         <v>43934.576504629629</v>
       </c>
@@ -25532,8 +27089,11 @@
       <c r="AN54">
         <v>0</v>
       </c>
+      <c r="AO54">
+        <v>20</v>
+      </c>
     </row>
-    <row r="55" spans="1:40">
+    <row r="55" spans="1:41">
       <c r="A55" s="1">
         <v>43935.556701388887</v>
       </c>
@@ -25654,8 +27214,11 @@
       <c r="AN55">
         <v>0</v>
       </c>
+      <c r="AO55">
+        <v>19</v>
+      </c>
     </row>
-    <row r="56" spans="1:40">
+    <row r="56" spans="1:41">
       <c r="A56" s="1">
         <v>43935.62605324074</v>
       </c>
@@ -25776,8 +27339,11 @@
       <c r="AN56">
         <v>1</v>
       </c>
+      <c r="AO56">
+        <v>11</v>
+      </c>
     </row>
-    <row r="57" spans="1:40">
+    <row r="57" spans="1:41">
       <c r="A57" s="1">
         <v>43936.641458333332</v>
       </c>
@@ -25898,8 +27464,11 @@
       <c r="AN57">
         <v>1</v>
       </c>
+      <c r="AO57">
+        <v>34</v>
+      </c>
     </row>
-    <row r="58" spans="1:40">
+    <row r="58" spans="1:41">
       <c r="A58" s="1">
         <v>43937.597881944443</v>
       </c>
@@ -26020,8 +27589,11 @@
       <c r="AN58">
         <v>1</v>
       </c>
+      <c r="AO58">
+        <v>35</v>
+      </c>
     </row>
-    <row r="59" spans="1:40">
+    <row r="59" spans="1:41">
       <c r="A59" s="1">
         <v>43938.590497685182</v>
       </c>
@@ -26142,8 +27714,11 @@
       <c r="AN59">
         <v>5</v>
       </c>
+      <c r="AO59">
+        <v>51</v>
+      </c>
     </row>
-    <row r="60" spans="1:40">
+    <row r="60" spans="1:41">
       <c r="A60" s="1">
         <v>43939.615011574075</v>
       </c>
@@ -26264,8 +27839,11 @@
       <c r="AN60">
         <v>2</v>
       </c>
+      <c r="AO60">
+        <v>49</v>
+      </c>
     </row>
-    <row r="61" spans="1:40">
+    <row r="61" spans="1:41">
       <c r="A61" s="1">
         <v>43940.66679398148</v>
       </c>
@@ -26386,8 +27964,11 @@
       <c r="AN61">
         <v>2</v>
       </c>
+      <c r="AO61">
+        <v>86</v>
+      </c>
     </row>
-    <row r="62" spans="1:40">
+    <row r="62" spans="1:41">
       <c r="A62" s="1">
         <v>43941.634942129633</v>
       </c>
@@ -26508,8 +28089,11 @@
       <c r="AN62">
         <v>1</v>
       </c>
+      <c r="AO62">
+        <v>38</v>
+      </c>
     </row>
-    <row r="63" spans="1:40">
+    <row r="63" spans="1:41">
       <c r="A63" s="1">
         <v>43942.651956018519</v>
       </c>
@@ -26630,8 +28214,11 @@
       <c r="AN63">
         <v>3</v>
       </c>
+      <c r="AO63">
+        <v>117</v>
+      </c>
     </row>
-    <row r="64" spans="1:40">
+    <row r="64" spans="1:41">
       <c r="A64" s="1">
         <v>43943.643599537034</v>
       </c>
@@ -26752,8 +28339,11 @@
       <c r="AN64">
         <v>3</v>
       </c>
+      <c r="AO64">
+        <v>91</v>
+      </c>
     </row>
-    <row r="65" spans="1:40">
+    <row r="65" spans="1:41">
       <c r="A65" s="1">
         <v>43944.657534722224</v>
       </c>
@@ -26874,8 +28464,11 @@
       <c r="AN65">
         <v>3</v>
       </c>
+      <c r="AO65">
+        <v>108</v>
+      </c>
     </row>
-    <row r="66" spans="1:40">
+    <row r="66" spans="1:41">
       <c r="A66" s="1">
         <v>43945.662118055552</v>
       </c>
@@ -26996,8 +28589,11 @@
       <c r="AN66">
         <v>1</v>
       </c>
+      <c r="AO66">
+        <v>114</v>
+      </c>
     </row>
-    <row r="67" spans="1:40">
+    <row r="67" spans="1:41">
       <c r="A67" s="1">
         <v>43946.66646990741</v>
       </c>
@@ -27118,8 +28714,11 @@
       <c r="AN67">
         <v>2</v>
       </c>
+      <c r="AO67">
+        <v>87</v>
+      </c>
     </row>
-    <row r="68" spans="1:40">
+    <row r="68" spans="1:41">
       <c r="A68" s="1">
         <v>43947.675543981481</v>
       </c>
@@ -27240,8 +28839,11 @@
       <c r="AN68">
         <v>5</v>
       </c>
+      <c r="AO68">
+        <v>86</v>
+      </c>
     </row>
-    <row r="69" spans="1:40">
+    <row r="69" spans="1:41">
       <c r="A69" s="1">
         <v>43948.650833333333</v>
       </c>
@@ -27362,8 +28964,11 @@
       <c r="AN69">
         <v>0</v>
       </c>
+      <c r="AO69">
+        <v>65</v>
+      </c>
     </row>
-    <row r="70" spans="1:40">
+    <row r="70" spans="1:41">
       <c r="A70" s="1">
         <v>43949.669594907406</v>
       </c>
@@ -27484,8 +29089,11 @@
       <c r="AN70">
         <v>4</v>
       </c>
+      <c r="AO70">
+        <v>195</v>
+      </c>
     </row>
-    <row r="71" spans="1:40">
+    <row r="71" spans="1:41">
       <c r="A71" s="1">
         <v>43950.665775462963</v>
       </c>
@@ -27606,8 +29214,11 @@
       <c r="AN71">
         <v>7</v>
       </c>
+      <c r="AO71">
+        <v>196</v>
+      </c>
     </row>
-    <row r="72" spans="1:40">
+    <row r="72" spans="1:41">
       <c r="A72" s="1">
         <v>43951.661261574074</v>
       </c>
@@ -27728,8 +29339,11 @@
       <c r="AN72">
         <v>7</v>
       </c>
+      <c r="AO72">
+        <v>204</v>
+      </c>
     </row>
-    <row r="73" spans="1:40">
+    <row r="73" spans="1:41">
       <c r="A73" s="1">
         <v>43952.629270833335</v>
       </c>
@@ -27850,8 +29464,11 @@
       <c r="AN73">
         <v>10</v>
       </c>
+      <c r="AO73">
+        <v>238</v>
+      </c>
     </row>
-    <row r="74" spans="1:40">
+    <row r="74" spans="1:41">
       <c r="A74" s="1">
         <v>43953.663969907408</v>
       </c>
@@ -27972,8 +29589,11 @@
       <c r="AN74">
         <v>17</v>
       </c>
+      <c r="AO74">
+        <v>220</v>
+      </c>
     </row>
-    <row r="75" spans="1:40">
+    <row r="75" spans="1:41">
       <c r="A75" s="1">
         <v>43954.667430555557</v>
       </c>
@@ -28094,8 +29714,11 @@
       <c r="AN75">
         <v>2</v>
       </c>
+      <c r="AO75">
+        <v>169</v>
+      </c>
     </row>
-    <row r="76" spans="1:40">
+    <row r="76" spans="1:41">
       <c r="A76" s="1">
         <v>43955.657326388886</v>
       </c>
@@ -28216,8 +29839,11 @@
       <c r="AN76">
         <v>6</v>
       </c>
+      <c r="AO76">
+        <v>245</v>
+      </c>
     </row>
-    <row r="77" spans="1:40">
+    <row r="77" spans="1:41">
       <c r="A77" s="1">
         <v>43956.6565162037</v>
       </c>
@@ -28338,8 +29964,11 @@
       <c r="AN77">
         <v>5</v>
       </c>
+      <c r="AO77">
+        <v>148</v>
+      </c>
     </row>
-    <row r="78" spans="1:40">
+    <row r="78" spans="1:41">
       <c r="A78" s="1">
         <v>43957.667824074073</v>
       </c>
@@ -28460,8 +30089,11 @@
       <c r="AN78">
         <v>5</v>
       </c>
+      <c r="AO78">
+        <v>195</v>
+      </c>
     </row>
-    <row r="79" spans="1:40">
+    <row r="79" spans="1:41">
       <c r="A79" s="1">
         <v>43958.639444444445</v>
       </c>
@@ -28582,8 +30214,11 @@
       <c r="AN79">
         <v>4</v>
       </c>
+      <c r="AO79">
+        <v>380</v>
+      </c>
     </row>
-    <row r="80" spans="1:40">
+    <row r="80" spans="1:41">
       <c r="A80" s="1">
         <v>43959.649583333332</v>
       </c>
@@ -28704,8 +30339,11 @@
       <c r="AN80">
         <v>10</v>
       </c>
+      <c r="AO80">
+        <v>386</v>
+      </c>
     </row>
-    <row r="81" spans="1:40">
+    <row r="81" spans="1:41">
       <c r="A81" s="1">
         <v>43960.633877314816</v>
       </c>
@@ -28826,8 +30464,11 @@
       <c r="AN81">
         <v>11</v>
       </c>
+      <c r="AO81">
+        <v>239</v>
+      </c>
     </row>
-    <row r="82" spans="1:40">
+    <row r="82" spans="1:41">
       <c r="A82" s="1">
         <v>43961.656747685185</v>
       </c>
@@ -28948,8 +30589,11 @@
       <c r="AN82">
         <v>15</v>
       </c>
+      <c r="AO82">
+        <v>248</v>
+      </c>
     </row>
-    <row r="83" spans="1:40">
+    <row r="83" spans="1:41">
       <c r="A83" s="1">
         <v>43962.656817129631</v>
       </c>
@@ -29070,8 +30714,11 @@
       <c r="AN83">
         <v>7</v>
       </c>
+      <c r="AO83">
+        <v>242</v>
+      </c>
     </row>
-    <row r="84" spans="1:40">
+    <row r="84" spans="1:41">
       <c r="A84" s="1">
         <v>43963.662939814814</v>
       </c>
@@ -29192,8 +30839,11 @@
       <c r="AN84">
         <v>8</v>
       </c>
+      <c r="AO84">
+        <v>146</v>
+      </c>
     </row>
-    <row r="85" spans="1:40">
+    <row r="85" spans="1:41">
       <c r="A85" s="1">
         <v>43964.645231481481</v>
       </c>
@@ -29314,8 +30964,11 @@
       <c r="AN85">
         <v>6</v>
       </c>
+      <c r="AO85">
+        <v>182</v>
+      </c>
     </row>
-    <row r="86" spans="1:40">
+    <row r="86" spans="1:41">
       <c r="A86" s="1">
         <v>43965.666458333333</v>
       </c>
@@ -29436,8 +31089,11 @@
       <c r="AN86">
         <v>3</v>
       </c>
+      <c r="AO86">
+        <v>189</v>
+      </c>
     </row>
-    <row r="87" spans="1:40">
+    <row r="87" spans="1:41">
       <c r="A87" s="1">
         <v>43966.657893518517</v>
       </c>
@@ -29558,8 +31214,11 @@
       <c r="AN87">
         <v>4</v>
       </c>
+      <c r="AO87">
+        <v>288</v>
+      </c>
     </row>
-    <row r="88" spans="1:40">
+    <row r="88" spans="1:41">
       <c r="A88" s="1">
         <v>43967.664201388892</v>
       </c>
@@ -29680,8 +31339,11 @@
       <c r="AN88">
         <v>5</v>
       </c>
+      <c r="AO88">
+        <v>176</v>
+      </c>
     </row>
-    <row r="89" spans="1:40">
+    <row r="89" spans="1:41">
       <c r="A89" s="1">
         <v>43968.632280092592</v>
       </c>
@@ -29802,8 +31464,11 @@
       <c r="AN89">
         <v>6</v>
       </c>
+      <c r="AO89">
+        <v>338</v>
+      </c>
     </row>
-    <row r="90" spans="1:40">
+    <row r="90" spans="1:41">
       <c r="A90" s="1">
         <v>43969.662060185183</v>
       </c>
@@ -29924,8 +31589,11 @@
       <c r="AN90">
         <v>9</v>
       </c>
+      <c r="AO90">
+        <v>208</v>
+      </c>
     </row>
-    <row r="91" spans="1:40">
+    <row r="91" spans="1:41">
       <c r="A91" s="1">
         <v>43970.65216435185</v>
       </c>
@@ -30046,8 +31714,11 @@
       <c r="AN91">
         <v>1</v>
       </c>
+      <c r="AO91">
+        <v>226</v>
+      </c>
     </row>
-    <row r="92" spans="1:40">
+    <row r="92" spans="1:41">
       <c r="A92" s="1">
         <v>43971.639363425929</v>
       </c>
@@ -30168,8 +31839,11 @@
       <c r="AN92">
         <v>8</v>
       </c>
+      <c r="AO92">
+        <v>284</v>
+      </c>
     </row>
-    <row r="93" spans="1:40">
+    <row r="93" spans="1:41">
       <c r="A93" s="1">
         <v>43972.658599537041</v>
       </c>
@@ -30290,8 +31964,11 @@
       <c r="AN93">
         <v>11</v>
       </c>
+      <c r="AO93">
+        <v>339</v>
+      </c>
     </row>
-    <row r="94" spans="1:40">
+    <row r="94" spans="1:41">
       <c r="A94" s="1">
         <v>43973.649317129632</v>
       </c>
@@ -30412,8 +32089,11 @@
       <c r="AN94">
         <v>10</v>
       </c>
+      <c r="AO94">
+        <v>245</v>
+      </c>
     </row>
-    <row r="95" spans="1:40">
+    <row r="95" spans="1:41">
       <c r="A95" s="1">
         <v>43974.66070601852</v>
       </c>
@@ -30534,8 +32214,11 @@
       <c r="AN95">
         <v>0</v>
       </c>
+      <c r="AO95">
+        <v>265</v>
+      </c>
     </row>
-    <row r="96" spans="1:40">
+    <row r="96" spans="1:41">
       <c r="A96" s="1">
         <v>43975.632037037038</v>
       </c>
@@ -30656,8 +32339,11 @@
       <c r="AN96">
         <v>5</v>
       </c>
+      <c r="AO96">
+        <v>313</v>
+      </c>
     </row>
-    <row r="97" spans="1:40">
+    <row r="97" spans="1:41">
       <c r="A97" s="1">
         <v>43976.648993055554</v>
       </c>
@@ -30778,8 +32464,11 @@
       <c r="AN97">
         <v>7</v>
       </c>
+      <c r="AO97">
+        <v>229</v>
+      </c>
     </row>
-    <row r="98" spans="1:40">
+    <row r="98" spans="1:41">
       <c r="A98" s="1">
         <v>43977.646331018521</v>
       </c>
@@ -30900,8 +32589,11 @@
       <c r="AN98">
         <v>16</v>
       </c>
+      <c r="AO98">
+        <v>276</v>
+      </c>
     </row>
-    <row r="99" spans="1:40">
+    <row r="99" spans="1:41">
       <c r="A99" s="1">
         <v>43978.655694444446</v>
       </c>
@@ -31022,8 +32714,11 @@
       <c r="AN99">
         <v>5</v>
       </c>
+      <c r="AO99">
+        <v>389</v>
+      </c>
     </row>
-    <row r="100" spans="1:40">
+    <row r="100" spans="1:41">
       <c r="A100" s="1">
         <v>43979.643958333334</v>
       </c>
@@ -31144,8 +32839,11 @@
       <c r="AN100">
         <v>5</v>
       </c>
+      <c r="AO100">
+        <v>182</v>
+      </c>
     </row>
-    <row r="101" spans="1:40">
+    <row r="101" spans="1:41">
       <c r="A101" s="1">
         <v>43980.656956018516</v>
       </c>
@@ -31266,8 +32964,11 @@
       <c r="AN101">
         <v>2</v>
       </c>
+      <c r="AO101">
+        <v>387</v>
+      </c>
     </row>
-    <row r="102" spans="1:40">
+    <row r="102" spans="1:41">
       <c r="A102" s="1">
         <v>43981.663819444446</v>
       </c>
@@ -31388,8 +33089,11 @@
       <c r="AN102">
         <v>12</v>
       </c>
+      <c r="AO102">
+        <v>553</v>
+      </c>
     </row>
-    <row r="103" spans="1:40">
+    <row r="103" spans="1:41">
       <c r="A103" s="1">
         <v>43982.643483796295</v>
       </c>
@@ -31510,8 +33214,11 @@
       <c r="AN103">
         <v>14</v>
       </c>
+      <c r="AO103">
+        <v>307</v>
+      </c>
     </row>
-    <row r="104" spans="1:40">
+    <row r="104" spans="1:41">
       <c r="A104" s="1">
         <v>43983.661226851851</v>
       </c>
@@ -31632,8 +33339,11 @@
       <c r="AN104">
         <v>12</v>
       </c>
+      <c r="AO104">
+        <v>416</v>
+      </c>
     </row>
-    <row r="105" spans="1:40">
+    <row r="105" spans="1:41">
       <c r="A105" s="1">
         <v>43984.658182870371</v>
       </c>
@@ -31754,8 +33464,11 @@
       <c r="AN105">
         <v>15</v>
       </c>
+      <c r="AO105">
+        <v>241</v>
+      </c>
     </row>
-    <row r="106" spans="1:40">
+    <row r="106" spans="1:41">
       <c r="A106" s="1">
         <v>43985.658182870371</v>
       </c>
@@ -31876,8 +33589,11 @@
       <c r="AN106">
         <v>1</v>
       </c>
+      <c r="AO106">
+        <v>348</v>
+      </c>
     </row>
-    <row r="107" spans="1:40">
+    <row r="107" spans="1:41">
       <c r="A107" s="1">
         <v>43986.655428240738</v>
       </c>
@@ -31998,8 +33714,11 @@
       <c r="AN107">
         <v>8</v>
       </c>
+      <c r="AO107">
+        <v>350</v>
+      </c>
     </row>
-    <row r="108" spans="1:40">
+    <row r="108" spans="1:41">
       <c r="A108" s="1">
         <v>43987.654479166667</v>
       </c>
@@ -32120,8 +33839,11 @@
       <c r="AN108">
         <v>10</v>
       </c>
+      <c r="AO108">
+        <v>328</v>
+      </c>
     </row>
-    <row r="109" spans="1:40">
+    <row r="109" spans="1:41">
       <c r="A109" s="1">
         <v>43988.651643518519</v>
       </c>
@@ -32242,8 +33964,11 @@
       <c r="AN109">
         <v>9</v>
       </c>
+      <c r="AO109">
+        <v>382</v>
+      </c>
     </row>
-    <row r="110" spans="1:40">
+    <row r="110" spans="1:41">
       <c r="A110" s="2">
         <v>43989.65902777778</v>
       </c>
@@ -32364,8 +34089,11 @@
       <c r="AN110" s="3">
         <v>12</v>
       </c>
+      <c r="AO110">
+        <v>260</v>
+      </c>
     </row>
-    <row r="111" spans="1:40">
+    <row r="111" spans="1:41">
       <c r="A111" s="1">
         <v>43990.653969907406</v>
       </c>
@@ -32486,8 +34214,11 @@
       <c r="AN111">
         <v>7</v>
       </c>
+      <c r="AO111">
+        <v>315</v>
+      </c>
     </row>
-    <row r="112" spans="1:40">
+    <row r="112" spans="1:41">
       <c r="A112" s="1">
         <v>43991.6565162037</v>
       </c>
@@ -32608,8 +34339,11 @@
       <c r="AN112">
         <v>4</v>
       </c>
+      <c r="AO112">
+        <v>663</v>
+      </c>
     </row>
-    <row r="113" spans="1:40">
+    <row r="113" spans="1:41">
       <c r="A113" s="1">
         <v>43992.661678240744</v>
       </c>
@@ -32730,8 +34464,11 @@
       <c r="AN113">
         <v>17</v>
       </c>
+      <c r="AO113">
+        <v>409</v>
+      </c>
     </row>
-    <row r="114" spans="1:40">
+    <row r="114" spans="1:41">
       <c r="A114" s="1">
         <v>43993.65861111111</v>
       </c>
@@ -32852,8 +34589,11 @@
       <c r="AN114">
         <v>5</v>
       </c>
+      <c r="AO114">
+        <v>681</v>
+      </c>
     </row>
-    <row r="115" spans="1:40">
+    <row r="115" spans="1:41">
       <c r="A115" s="1">
         <v>43994.655590277776</v>
       </c>
@@ -32974,8 +34714,11 @@
       <c r="AN115">
         <v>12</v>
       </c>
+      <c r="AO115">
+        <v>627</v>
+      </c>
     </row>
-    <row r="116" spans="1:40">
+    <row r="116" spans="1:41">
       <c r="A116" s="1">
         <v>43995.654722222222</v>
       </c>
@@ -33096,8 +34839,11 @@
       <c r="AN116">
         <v>8</v>
       </c>
+      <c r="AO116">
+        <v>501</v>
+      </c>
     </row>
-    <row r="117" spans="1:40">
+    <row r="117" spans="1:41">
       <c r="A117" s="1">
         <v>43996.655335648145</v>
       </c>
@@ -33218,8 +34964,11 @@
       <c r="AN117">
         <v>13</v>
       </c>
+      <c r="AO117">
+        <v>403</v>
+      </c>
     </row>
-    <row r="118" spans="1:40">
+    <row r="118" spans="1:41">
       <c r="A118" s="1">
         <v>43997.66034722222</v>
       </c>
@@ -33340,8 +35089,11 @@
       <c r="AN118">
         <v>4</v>
       </c>
+      <c r="AO118">
+        <v>573</v>
+      </c>
     </row>
-    <row r="119" spans="1:40">
+    <row r="119" spans="1:41">
       <c r="A119" s="1">
         <v>43998.66715277778</v>
       </c>
@@ -33462,8 +35214,11 @@
       <c r="AN119">
         <v>31</v>
       </c>
+      <c r="AO119">
+        <v>490</v>
+      </c>
     </row>
-    <row r="120" spans="1:40">
+    <row r="120" spans="1:41">
       <c r="A120" s="1">
         <v>43999.637974537036</v>
       </c>
@@ -33584,8 +35339,11 @@
       <c r="AN120">
         <v>14</v>
       </c>
+      <c r="AO120">
+        <v>587</v>
+      </c>
     </row>
-    <row r="121" spans="1:40">
+    <row r="121" spans="1:41">
       <c r="A121" s="1">
         <v>44000.655023148145</v>
       </c>
@@ -33706,8 +35464,11 @@
       <c r="AN121">
         <v>6</v>
       </c>
+      <c r="AO121">
+        <v>745</v>
+      </c>
     </row>
-    <row r="122" spans="1:40">
+    <row r="122" spans="1:41">
       <c r="A122" s="1">
         <v>44001.628831018519</v>
       </c>
@@ -33828,8 +35589,11 @@
       <c r="AN122">
         <v>12</v>
       </c>
+      <c r="AO122">
+        <v>667</v>
+      </c>
     </row>
-    <row r="123" spans="1:40">
+    <row r="123" spans="1:41">
       <c r="A123" s="1">
         <v>44002.645497685182</v>
       </c>
@@ -33950,8 +35714,11 @@
       <c r="AN123">
         <v>19</v>
       </c>
+      <c r="AO123">
+        <v>661</v>
+      </c>
     </row>
-    <row r="124" spans="1:40">
+    <row r="124" spans="1:41">
       <c r="A124" s="1">
         <v>44003.648101851853</v>
       </c>
@@ -34072,8 +35839,11 @@
       <c r="AN124">
         <v>12</v>
       </c>
+      <c r="AO124">
+        <v>436</v>
+      </c>
     </row>
-    <row r="125" spans="1:40">
+    <row r="125" spans="1:41">
       <c r="A125" s="1">
         <v>44004.63486111111</v>
       </c>
@@ -34194,8 +35964,11 @@
       <c r="AN125">
         <v>7</v>
       </c>
+      <c r="AO125">
+        <v>675</v>
+      </c>
     </row>
-    <row r="126" spans="1:40">
+    <row r="126" spans="1:41">
       <c r="A126" s="1">
         <v>44005.646134259259</v>
       </c>
@@ -34316,8 +36089,11 @@
       <c r="AN126">
         <v>8</v>
       </c>
+      <c r="AO126">
+        <v>452</v>
+      </c>
     </row>
-    <row r="127" spans="1:40">
+    <row r="127" spans="1:41">
       <c r="A127" s="1">
         <v>44006.641284722224</v>
       </c>
@@ -34438,8 +36214,11 @@
       <c r="AN127">
         <v>9</v>
       </c>
+      <c r="AO127">
+        <v>649</v>
+      </c>
     </row>
-    <row r="128" spans="1:40">
+    <row r="128" spans="1:41">
       <c r="A128" s="1">
         <v>44007.658310185187</v>
       </c>
@@ -34560,8 +36339,11 @@
       <c r="AN128">
         <v>7</v>
       </c>
+      <c r="AO128">
+        <v>594</v>
+      </c>
     </row>
-    <row r="129" spans="1:40">
+    <row r="129" spans="1:41">
       <c r="A129" s="1">
         <v>44008.659884259258</v>
       </c>
@@ -34681,6 +36463,9 @@
       </c>
       <c r="AN129">
         <v>5</v>
+      </c>
+      <c r="AO129">
+        <v>684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:repeat: update data day 165
</commit_message>
<xml_diff>
--- a/covid19Naija/data/records_covid19.xlsx
+++ b/covid19Naija/data/records_covid19.xlsx
@@ -460,8 +460,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="209">
+  <cellStyleXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -677,7 +679,7 @@
     <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="209">
+  <cellStyles count="211">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -782,6 +784,7 @@
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -886,6 +889,7 @@
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1217,9 +1221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI178" sqref="AI178"/>
+      <selection pane="bottomLeft" activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20500,7 +20504,7 @@
         <v>12</v>
       </c>
       <c r="AO153">
-        <f t="shared" ref="AO153:AO165" si="2">SUM(B153:AL153)</f>
+        <f t="shared" ref="AO153:AO166" si="2">SUM(B153:AL153)</f>
         <v>562</v>
       </c>
     </row>
@@ -22017,24 +22021,26 @@
       </c>
     </row>
     <row r="166" spans="1:41">
-      <c r="A166" s="1"/>
+      <c r="A166" s="1">
+        <v>44045.643576388888</v>
+      </c>
       <c r="B166">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D166">
         <v>0</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F166">
         <v>0</v>
       </c>
       <c r="G166">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H166">
         <v>0</v>
@@ -22043,7 +22049,7 @@
         <v>0</v>
       </c>
       <c r="J166">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K166">
         <v>0</v>
@@ -22058,19 +22064,19 @@
         <v>0</v>
       </c>
       <c r="O166">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="P166">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Q166">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R166">
         <v>0</v>
       </c>
       <c r="S166">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="T166">
         <v>0</v>
@@ -22082,7 +22088,7 @@
         <v>0</v>
       </c>
       <c r="W166">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="X166">
         <v>0</v>
@@ -22091,7 +22097,7 @@
         <v>0</v>
       </c>
       <c r="Z166">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA166">
         <v>0</v>
@@ -22100,7 +22106,7 @@
         <v>0</v>
       </c>
       <c r="AC166">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD166">
         <v>0</v>
@@ -22112,7 +22118,7 @@
         <v>0</v>
       </c>
       <c r="AG166">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AH166">
         <v>0</v>
@@ -22124,16 +22130,20 @@
         <v>0</v>
       </c>
       <c r="AK166">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AL166">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AM166">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="AN166">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AO166">
+        <f t="shared" si="2"/>
+        <v>304</v>
       </c>
     </row>
     <row r="167" spans="1:41">
@@ -22978,11 +22988,11 @@
     <row r="174" spans="1:41">
       <c r="B174">
         <f>SUM(B2:B173)</f>
-        <v>15186</v>
+        <v>15267</v>
       </c>
       <c r="C174">
         <f t="shared" ref="C174:AN174" si="3">SUM(C2:C173)</f>
-        <v>3933</v>
+        <v>3972</v>
       </c>
       <c r="D174">
         <f t="shared" si="3"/>
@@ -22990,7 +23000,7 @@
       </c>
       <c r="E174">
         <f t="shared" si="3"/>
-        <v>1397</v>
+        <v>1403</v>
       </c>
       <c r="F174">
         <f t="shared" si="3"/>
@@ -22998,7 +23008,7 @@
       </c>
       <c r="G174">
         <f t="shared" si="3"/>
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="H174">
         <f t="shared" si="3"/>
@@ -23010,7 +23020,7 @@
       </c>
       <c r="J174">
         <f t="shared" si="3"/>
-        <v>2300</v>
+        <v>2311</v>
       </c>
       <c r="K174">
         <f t="shared" si="3"/>
@@ -23030,15 +23040,15 @@
       </c>
       <c r="O174">
         <f t="shared" si="3"/>
-        <v>1457</v>
+        <v>1481</v>
       </c>
       <c r="P174">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="Q174">
         <f t="shared" si="3"/>
-        <v>1192</v>
+        <v>1204</v>
       </c>
       <c r="R174">
         <f t="shared" si="3"/>
@@ -23046,7 +23056,7 @@
       </c>
       <c r="S174">
         <f t="shared" si="3"/>
-        <v>1806</v>
+        <v>1829</v>
       </c>
       <c r="T174">
         <f t="shared" si="3"/>
@@ -23062,7 +23072,7 @@
       </c>
       <c r="W174">
         <f t="shared" si="3"/>
-        <v>551</v>
+        <v>582</v>
       </c>
       <c r="X174">
         <f t="shared" si="3"/>
@@ -23074,7 +23084,7 @@
       </c>
       <c r="Z174">
         <f t="shared" si="3"/>
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="AA174">
         <f t="shared" si="3"/>
@@ -23086,7 +23096,7 @@
       </c>
       <c r="AC174">
         <f t="shared" si="3"/>
-        <v>1211</v>
+        <v>1227</v>
       </c>
       <c r="AD174">
         <f t="shared" si="3"/>
@@ -23102,7 +23112,7 @@
       </c>
       <c r="AG174">
         <f t="shared" si="3"/>
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="AH174">
         <f t="shared" si="3"/>
@@ -23118,25 +23128,25 @@
       </c>
       <c r="AK174">
         <f t="shared" si="3"/>
-        <v>796</v>
+        <v>808</v>
       </c>
       <c r="AL174">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="AM174">
         <f t="shared" si="3"/>
-        <v>20087</v>
+        <v>20308</v>
       </c>
       <c r="AN174">
         <f t="shared" si="3"/>
-        <v>883</v>
+        <v>888</v>
       </c>
     </row>
     <row r="177" spans="42:42">
       <c r="AP177">
-        <f>SUM(AO2:AO165)</f>
-        <v>43544</v>
+        <f>SUM(AO2:AO166)</f>
+        <v>43848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
source data for map
</commit_message>
<xml_diff>
--- a/covid19Naija/data/records_covid19.xlsx
+++ b/covid19Naija/data/records_covid19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/covid19Naija/covid19Naija/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F839148-3593-4E4B-A1F3-E7A5BFA1A92C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26547985-5C67-C444-B576-9A1FAB0CFC50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="3760" windowWidth="25360" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2060" yWindow="460" windowWidth="25360" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="records" sheetId="1" r:id="rId1"/>
@@ -1290,9 +1290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A244" sqref="A244:AO244"/>
+      <selection pane="bottomLeft" activeCell="AJ248" sqref="AJ248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20573,7 +20573,7 @@
         <v>12</v>
       </c>
       <c r="AO153">
-        <f t="shared" ref="AO153:AO244" si="2">SUM(B153:AL153)</f>
+        <f t="shared" ref="AO153:AO246" si="2">SUM(B153:AL153)</f>
         <v>562</v>
       </c>
     </row>
@@ -32044,18 +32044,20 @@
       </c>
     </row>
     <row r="245" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A245" s="1"/>
+      <c r="A245" s="1">
+        <v>44124.63958333333</v>
+      </c>
       <c r="B245">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C245">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D245">
         <v>0</v>
       </c>
       <c r="E245">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F245">
         <v>0</v>
@@ -32085,19 +32087,19 @@
         <v>0</v>
       </c>
       <c r="O245">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P245">
         <v>0</v>
       </c>
       <c r="Q245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R245">
         <v>0</v>
       </c>
       <c r="S245">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T245">
         <v>0</v>
@@ -32161,10 +32163,16 @@
       </c>
       <c r="AN245">
         <v>0</v>
+      </c>
+      <c r="AO245">
+        <f t="shared" si="2"/>
+        <v>48</v>
       </c>
     </row>
     <row r="246" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A246" s="1"/>
+      <c r="A246" s="1">
+        <v>44125.63958333333</v>
+      </c>
       <c r="B246">
         <v>0</v>
       </c>
@@ -32211,7 +32219,7 @@
         <v>0</v>
       </c>
       <c r="Q246">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R246">
         <v>0</v>
@@ -32280,11 +32288,16 @@
         <v>0</v>
       </c>
       <c r="AN246">
+        <v>0</v>
+      </c>
+      <c r="AO246">
         <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A247" s="1"/>
+      <c r="A247" s="1">
+        <v>44126.63958333333</v>
+      </c>
       <c r="B247">
         <v>0</v>
       </c>
@@ -32400,11 +32413,16 @@
         <v>0</v>
       </c>
       <c r="AN247">
+        <v>0</v>
+      </c>
+      <c r="AO247">
         <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A248" s="1"/>
+      <c r="A248" s="1">
+        <v>44127.63958333333</v>
+      </c>
       <c r="B248">
         <v>0</v>
       </c>
@@ -32520,11 +32538,16 @@
         <v>0</v>
       </c>
       <c r="AN248">
+        <v>0</v>
+      </c>
+      <c r="AO248">
         <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A249" s="1"/>
+      <c r="A249" s="1">
+        <v>44128.63958333333</v>
+      </c>
       <c r="B249">
         <v>0</v>
       </c>
@@ -32644,7 +32667,9 @@
       </c>
     </row>
     <row r="250" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A250" s="1"/>
+      <c r="A250" s="1">
+        <v>44123.63958333333</v>
+      </c>
       <c r="B250">
         <v>0</v>
       </c>
@@ -32764,7 +32789,9 @@
       </c>
     </row>
     <row r="251" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A251" s="1"/>
+      <c r="A251" s="1">
+        <v>44123.63958333333</v>
+      </c>
       <c r="B251">
         <v>0</v>
       </c>
@@ -32884,7 +32911,9 @@
       </c>
     </row>
     <row r="252" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A252" s="1"/>
+      <c r="A252" s="1">
+        <v>44123.63958333333</v>
+      </c>
       <c r="B252">
         <v>0</v>
       </c>
@@ -33004,7 +33033,9 @@
       </c>
     </row>
     <row r="253" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A253" s="1"/>
+      <c r="A253" s="1">
+        <v>44123.63958333333</v>
+      </c>
       <c r="B253">
         <v>0</v>
       </c>
@@ -33124,7 +33155,9 @@
       </c>
     </row>
     <row r="254" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A254" s="1"/>
+      <c r="A254" s="1">
+        <v>44123.63958333333</v>
+      </c>
       <c r="B254">
         <v>0</v>
       </c>
@@ -33366,11 +33399,11 @@
     <row r="256" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B256">
         <f t="shared" ref="B256:AN256" si="3">SUM(B2:B255)</f>
-        <v>20708</v>
+        <v>20726</v>
       </c>
       <c r="C256">
         <f t="shared" si="3"/>
-        <v>5911</v>
+        <v>5924</v>
       </c>
       <c r="D256">
         <f t="shared" si="3"/>
@@ -33378,7 +33411,7 @@
       </c>
       <c r="E256">
         <f t="shared" si="3"/>
-        <v>1976</v>
+        <v>1981</v>
       </c>
       <c r="F256">
         <f t="shared" si="3"/>
@@ -33418,7 +33451,7 @@
       </c>
       <c r="O256">
         <f t="shared" si="3"/>
-        <v>2562</v>
+        <v>2568</v>
       </c>
       <c r="P256">
         <f t="shared" si="3"/>
@@ -33426,7 +33459,7 @@
       </c>
       <c r="Q256">
         <f t="shared" si="3"/>
-        <v>1657</v>
+        <v>1659</v>
       </c>
       <c r="R256">
         <f t="shared" si="3"/>
@@ -33434,7 +33467,7 @@
       </c>
       <c r="S256">
         <f t="shared" si="3"/>
-        <v>2735</v>
+        <v>2740</v>
       </c>
       <c r="T256">
         <f t="shared" si="3"/>

</xml_diff>